<commit_message>
retake of the article
</commit_message>
<xml_diff>
--- a/data/datos antropométricos y cardiovasculares.xlsx
+++ b/data/datos antropométricos y cardiovasculares.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Proyectos I+D+i 2016_BEBESANO\BEBESANO CRONICO\Resultados estudio cronico bebesano\Resultados definitivos para la estadística\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristina García\Documents\Proyectos\1stStepsPhD\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
         <v>27.9</v>
       </c>
       <c r="H2" s="3">
-        <f>G2-F2</f>
+        <f t="shared" ref="H2:H33" si="0">G2-F2</f>
         <v>-0.10000000000000142</v>
       </c>
       <c r="I2" s="3">
@@ -617,7 +617,7 @@
         <v>69.8</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D66" si="1">C3-B3</f>
         <v>-0.40000000000000568</v>
       </c>
       <c r="E3" s="3">
@@ -630,7 +630,7 @@
         <v>27.3</v>
       </c>
       <c r="H3" s="3">
-        <f>G3-F3</f>
+        <f t="shared" si="0"/>
         <v>-9.9999999999997868E-2</v>
       </c>
       <c r="I3" s="3">
@@ -640,7 +640,7 @@
         <v>35.4</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K66" si="1">J3-I3</f>
+        <f t="shared" ref="K3:K66" si="2">J3-I3</f>
         <v>-3.2000000000000028</v>
       </c>
       <c r="L3" s="3">
@@ -679,7 +679,7 @@
         <v>76.2</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.2000000000000028</v>
       </c>
       <c r="E4" s="3">
@@ -692,7 +692,7 @@
         <v>25.8</v>
       </c>
       <c r="H4" s="3">
-        <f>G4-F4</f>
+        <f t="shared" si="0"/>
         <v>-1.0999999999999979</v>
       </c>
       <c r="I4" s="3">
@@ -702,7 +702,7 @@
         <v>36.799999999999997</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.4000000000000057</v>
       </c>
       <c r="L4" s="3">
@@ -741,7 +741,7 @@
         <v>80.3</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="E5" s="3">
@@ -754,7 +754,7 @@
         <v>29.5</v>
       </c>
       <c r="H5" s="3">
-        <f>G5-F5</f>
+        <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
       <c r="I5" s="3">
@@ -764,7 +764,7 @@
         <v>41.2</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L5" s="3">
@@ -801,7 +801,7 @@
         <v>70.3</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.10000000000000853</v>
       </c>
       <c r="E6" s="3">
@@ -814,7 +814,7 @@
         <v>24.9</v>
       </c>
       <c r="H6" s="3">
-        <f>G6-F6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I6" s="3">
@@ -824,7 +824,7 @@
         <v>31.1</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.8999999999999986</v>
       </c>
       <c r="L6" s="3">
@@ -863,7 +863,7 @@
         <v>89.1</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3999999999999915</v>
       </c>
       <c r="E7" s="3">
@@ -876,7 +876,7 @@
         <v>24.7</v>
       </c>
       <c r="H7" s="3">
-        <f>G7-F7</f>
+        <f t="shared" si="0"/>
         <v>0.39999999999999858</v>
       </c>
       <c r="I7" s="3">
@@ -886,7 +886,7 @@
         <v>23.6</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.8999999999999986</v>
       </c>
       <c r="L7" s="3">
@@ -925,7 +925,7 @@
         <v>78.5</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.0999999999999943</v>
       </c>
       <c r="E8" s="3">
@@ -938,7 +938,7 @@
         <v>26.2</v>
       </c>
       <c r="H8" s="3">
-        <f>G8-F8</f>
+        <f t="shared" si="0"/>
         <v>-0.40000000000000213</v>
       </c>
       <c r="I8" s="3">
@@ -948,7 +948,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.1000000000000014</v>
       </c>
       <c r="L8" s="3">
@@ -987,7 +987,7 @@
         <v>67.8</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E9" s="3">
@@ -1000,7 +1000,7 @@
         <v>25.2</v>
       </c>
       <c r="H9" s="3">
-        <f>G9-F9</f>
+        <f t="shared" si="0"/>
         <v>9.9999999999997868E-2</v>
       </c>
       <c r="I9" s="3">
@@ -1010,7 +1010,7 @@
         <v>39.1</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="L9" s="3">
@@ -1049,7 +1049,7 @@
         <v>64.8</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9999999999994316E-2</v>
       </c>
       <c r="E10" s="3">
@@ -1062,7 +1062,7 @@
         <v>28</v>
       </c>
       <c r="H10" s="3">
-        <f>G10-F10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I10" s="3">
@@ -1072,7 +1072,7 @@
         <v>43.7</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
       <c r="L10" s="3">
@@ -1111,7 +1111,7 @@
         <v>89.9</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3999999999999915</v>
       </c>
       <c r="E11" s="3">
@@ -1124,7 +1124,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="H11" s="3">
-        <f>G11-F11</f>
+        <f t="shared" si="0"/>
         <v>-0.40000000000000568</v>
       </c>
       <c r="I11" s="3">
@@ -1134,7 +1134,7 @@
         <v>43.1</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.1000000000000014</v>
       </c>
       <c r="L11" s="3">
@@ -1173,7 +1173,7 @@
         <v>82.4</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.89999999999999147</v>
       </c>
       <c r="E12" s="3">
@@ -1186,7 +1186,7 @@
         <v>30.3</v>
       </c>
       <c r="H12" s="3">
-        <f>G12-F12</f>
+        <f t="shared" si="0"/>
         <v>-0.19999999999999929</v>
       </c>
       <c r="I12" s="3">
@@ -1196,7 +1196,7 @@
         <v>45.4</v>
       </c>
       <c r="K12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="L12" s="3">
@@ -1233,7 +1233,7 @@
         <v>71.900000000000006</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10000000000000853</v>
       </c>
       <c r="E13" s="5">
@@ -1246,7 +1246,7 @@
         <v>24.9</v>
       </c>
       <c r="H13" s="3">
-        <f>G13-F13</f>
+        <f t="shared" si="0"/>
         <v>9.9999999999997868E-2</v>
       </c>
       <c r="I13" s="3">
@@ -1256,7 +1256,7 @@
         <v>34.700000000000003</v>
       </c>
       <c r="K13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.59999999999999432</v>
       </c>
       <c r="L13" s="3">
@@ -1295,7 +1295,7 @@
         <v>86.6</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6999999999999886</v>
       </c>
       <c r="E14" s="3">
@@ -1308,7 +1308,7 @@
         <v>31.8</v>
       </c>
       <c r="H14" s="3">
-        <f>G14-F14</f>
+        <f t="shared" si="0"/>
         <v>1.3000000000000007</v>
       </c>
       <c r="I14" s="3">
@@ -1318,7 +1318,7 @@
         <v>44.3</v>
       </c>
       <c r="K14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="L14" s="3">
@@ -1355,7 +1355,7 @@
         <v>73.900000000000006</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="E15" s="3">
@@ -1368,7 +1368,7 @@
         <v>27.1</v>
       </c>
       <c r="H15" s="3">
-        <f>G15-F15</f>
+        <f t="shared" si="0"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="I15" s="3">
@@ -1378,7 +1378,7 @@
         <v>36.9</v>
       </c>
       <c r="K15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.2000000000000028</v>
       </c>
       <c r="L15" s="3">
@@ -1417,7 +1417,7 @@
         <v>79.3</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5999999999999943</v>
       </c>
       <c r="E16" s="5">
@@ -1430,7 +1430,7 @@
         <v>31</v>
       </c>
       <c r="H16" s="3">
-        <f>G16-F16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I16" s="3">
@@ -1440,7 +1440,7 @@
         <v>43.6</v>
       </c>
       <c r="K16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="L16" s="3">
@@ -1479,7 +1479,7 @@
         <v>85</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.9000000000000057</v>
       </c>
       <c r="E17" s="3">
@@ -1492,7 +1492,7 @@
         <v>30.8</v>
       </c>
       <c r="H17" s="3">
-        <f>G17-F17</f>
+        <f t="shared" si="0"/>
         <v>-0.69999999999999929</v>
       </c>
       <c r="I17" s="3">
@@ -1502,7 +1502,7 @@
         <v>44.7</v>
       </c>
       <c r="K17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2000000000000028</v>
       </c>
       <c r="L17" s="3">
@@ -1539,7 +1539,7 @@
         <v>66.400000000000006</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.5999999999999943</v>
       </c>
       <c r="E18" s="3">
@@ -1552,7 +1552,7 @@
         <v>24.4</v>
       </c>
       <c r="H18" s="3">
-        <f>G18-F18</f>
+        <f t="shared" si="0"/>
         <v>-0.90000000000000213</v>
       </c>
       <c r="I18" s="3">
@@ -1562,7 +1562,7 @@
         <v>36.1</v>
       </c>
       <c r="K18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1000000000000014</v>
       </c>
       <c r="L18" s="3">
@@ -1601,7 +1601,7 @@
         <v>68.7</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.7000000000000028</v>
       </c>
       <c r="E19" s="3">
@@ -1614,7 +1614,7 @@
         <v>22.2</v>
       </c>
       <c r="H19" s="3">
-        <f>G19-F19</f>
+        <f t="shared" si="0"/>
         <v>-0.60000000000000142</v>
       </c>
       <c r="I19" s="3">
@@ -1624,7 +1624,7 @@
         <v>33.6</v>
       </c>
       <c r="K19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.5</v>
       </c>
       <c r="L19" s="3">
@@ -1663,7 +1663,7 @@
         <v>61.9</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.70000000000000284</v>
       </c>
       <c r="E20" s="3">
@@ -1676,7 +1676,7 @@
         <v>23</v>
       </c>
       <c r="H20" s="3">
-        <f>G20-F20</f>
+        <f t="shared" si="0"/>
         <v>-0.30000000000000071</v>
       </c>
       <c r="I20" s="3">
@@ -1686,7 +1686,7 @@
         <v>29.2</v>
       </c>
       <c r="K20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L20" s="3">
@@ -1725,7 +1725,7 @@
         <v>57.9</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.7000000000000028</v>
       </c>
       <c r="E21" s="3">
@@ -1738,7 +1738,7 @@
         <v>24.1</v>
       </c>
       <c r="H21" s="3">
-        <f>G21-F21</f>
+        <f t="shared" si="0"/>
         <v>-0.69999999999999929</v>
       </c>
       <c r="I21" s="3">
@@ -1748,7 +1748,7 @@
         <v>34.4</v>
       </c>
       <c r="K21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.5</v>
       </c>
       <c r="L21" s="3">
@@ -1787,7 +1787,7 @@
         <v>95.5</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9000000000000057</v>
       </c>
       <c r="E22" s="3">
@@ -1800,7 +1800,7 @@
         <v>28.5</v>
       </c>
       <c r="H22" s="3">
-        <f>G22-F22</f>
+        <f t="shared" si="0"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I22" s="3">
@@ -1810,7 +1810,7 @@
         <v>26.7</v>
       </c>
       <c r="K22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.1000000000000014</v>
       </c>
       <c r="L22" s="3">
@@ -1849,22 +1849,22 @@
         <v>87.6</v>
       </c>
       <c r="D23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1.78</v>
+      </c>
+      <c r="F23" s="3">
+        <v>27.6</v>
+      </c>
+      <c r="G23" s="3">
+        <v>27.6</v>
+      </c>
+      <c r="H23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="3">
-        <v>1.78</v>
-      </c>
-      <c r="F23" s="3">
-        <v>27.6</v>
-      </c>
-      <c r="G23" s="3">
-        <v>27.6</v>
-      </c>
-      <c r="H23" s="3">
-        <f>G23-F23</f>
-        <v>0</v>
-      </c>
       <c r="I23" s="3">
         <v>23</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>18.8</v>
       </c>
       <c r="K23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.1999999999999993</v>
       </c>
       <c r="L23" s="3">
@@ -1924,7 +1924,7 @@
         <v>25.9</v>
       </c>
       <c r="H24" s="3">
-        <f>G24-F24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" s="3">
@@ -1934,7 +1934,7 @@
         <v>23.5</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.3999999999999986</v>
       </c>
       <c r="L24" s="3">
@@ -1986,7 +1986,7 @@
         <v>25.8</v>
       </c>
       <c r="H25" s="3">
-        <f>G25-F25</f>
+        <f t="shared" si="0"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="I25" s="3">
@@ -1996,7 +1996,7 @@
         <v>21.2</v>
       </c>
       <c r="K25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.6000000000000014</v>
       </c>
       <c r="L25" s="3">
@@ -2035,7 +2035,7 @@
         <v>72.5</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.7000000000000028</v>
       </c>
       <c r="E26" s="3">
@@ -2048,7 +2048,7 @@
         <v>25</v>
       </c>
       <c r="H26" s="3">
-        <f>G26-F26</f>
+        <f t="shared" si="0"/>
         <v>-0.69999999999999929</v>
       </c>
       <c r="I26" s="3">
@@ -2058,7 +2058,7 @@
         <v>17.2</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.6999999999999993</v>
       </c>
       <c r="L26" s="3">
@@ -2097,7 +2097,7 @@
         <v>87.1</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="E27" s="3">
@@ -2110,7 +2110,7 @@
         <v>27.2</v>
       </c>
       <c r="H27" s="3">
-        <f>G27-F27</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="I27" s="3">
@@ -2120,7 +2120,7 @@
         <v>24.6</v>
       </c>
       <c r="K27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6999999999999993</v>
       </c>
       <c r="L27" s="3">
@@ -2159,7 +2159,7 @@
         <v>101.6</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.7000000000000028</v>
       </c>
       <c r="E28" s="3">
@@ -2172,7 +2172,7 @@
         <v>29.7</v>
       </c>
       <c r="H28" s="3">
-        <f>G28-F28</f>
+        <f t="shared" si="0"/>
         <v>-1.4000000000000021</v>
       </c>
       <c r="I28" s="3">
@@ -2182,7 +2182,7 @@
         <v>21.4</v>
       </c>
       <c r="K28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.6000000000000014</v>
       </c>
       <c r="L28" s="3">
@@ -2221,7 +2221,7 @@
         <v>77.7</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3999999999999915</v>
       </c>
       <c r="E29" s="3">
@@ -2234,7 +2234,7 @@
         <v>25.4</v>
       </c>
       <c r="H29" s="3">
-        <f>G29-F29</f>
+        <f t="shared" si="0"/>
         <v>-0.40000000000000213</v>
       </c>
       <c r="I29" s="3">
@@ -2244,7 +2244,7 @@
         <v>23.2</v>
       </c>
       <c r="K29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.1999999999999993</v>
       </c>
       <c r="L29" s="3">
@@ -2283,7 +2283,7 @@
         <v>87.9</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.7999999999999972</v>
       </c>
       <c r="E30" s="3">
@@ -2296,7 +2296,7 @@
         <v>26.2</v>
       </c>
       <c r="H30" s="3">
-        <f>G30-F30</f>
+        <f t="shared" si="0"/>
         <v>-2.6999999999999993</v>
       </c>
       <c r="I30" s="3">
@@ -2306,7 +2306,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="K30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-8.8999999999999986</v>
       </c>
       <c r="L30" s="3">
@@ -2345,7 +2345,7 @@
         <v>85.4</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.0999999999999943</v>
       </c>
       <c r="E31" s="3">
@@ -2358,7 +2358,7 @@
         <v>26.6</v>
       </c>
       <c r="H31" s="3">
-        <f>G31-F31</f>
+        <f t="shared" si="0"/>
         <v>-6.7999999999999972</v>
       </c>
       <c r="I31" s="3">
@@ -2368,7 +2368,7 @@
         <v>29</v>
       </c>
       <c r="K31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
       <c r="L31" s="3">
@@ -2407,7 +2407,7 @@
         <v>91.5</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E32" s="3">
@@ -2420,7 +2420,7 @@
         <v>28.2</v>
       </c>
       <c r="H32" s="3">
-        <f>G32-F32</f>
+        <f t="shared" si="0"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="I32" s="3">
@@ -2430,7 +2430,7 @@
         <v>21.5</v>
       </c>
       <c r="K32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.1000000000000014</v>
       </c>
       <c r="L32" s="3">
@@ -2469,7 +2469,7 @@
         <v>100.5</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.59999999999999432</v>
       </c>
       <c r="E33" s="3">
@@ -2482,7 +2482,7 @@
         <v>31</v>
       </c>
       <c r="H33" s="3">
-        <f>G33-F33</f>
+        <f t="shared" si="0"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I33" s="3">
@@ -2492,7 +2492,7 @@
         <v>26.1</v>
       </c>
       <c r="K33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.6999999999999993</v>
       </c>
       <c r="L33" s="3">
@@ -2531,7 +2531,7 @@
         <v>89.2</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.59999999999999432</v>
       </c>
       <c r="E34" s="3">
@@ -2544,7 +2544,7 @@
         <v>29.5</v>
       </c>
       <c r="H34" s="3">
-        <f>G34-F34</f>
+        <f t="shared" ref="H34:H65" si="3">G34-F34</f>
         <v>-0.19999999999999929</v>
       </c>
       <c r="I34" s="3">
@@ -2554,7 +2554,7 @@
         <v>28.5</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="L34" s="3">
@@ -2593,7 +2593,7 @@
         <v>92.3</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E35" s="3">
@@ -2606,7 +2606,7 @@
         <v>31.9</v>
       </c>
       <c r="H35" s="3">
-        <f>G35-F35</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I35" s="3">
@@ -2616,7 +2616,7 @@
         <v>28.3</v>
       </c>
       <c r="K35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.19999999999999929</v>
       </c>
       <c r="L35" s="3">
@@ -2655,7 +2655,7 @@
         <v>94.3</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="E36" s="3">
@@ -2668,7 +2668,7 @@
         <v>29.1</v>
       </c>
       <c r="H36" s="3">
-        <f>G36-F36</f>
+        <f t="shared" si="3"/>
         <v>-1.1999999999999993</v>
       </c>
       <c r="I36" s="3">
@@ -2678,7 +2678,7 @@
         <v>26</v>
       </c>
       <c r="K36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.1999999999999993</v>
       </c>
       <c r="L36" s="3">
@@ -2717,7 +2717,7 @@
         <v>85.8</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.60000000000000853</v>
       </c>
       <c r="E37" s="3">
@@ -2730,7 +2730,7 @@
         <v>26.5</v>
       </c>
       <c r="H37" s="3">
-        <f>G37-F37</f>
+        <f t="shared" si="3"/>
         <v>-0.19999999999999929</v>
       </c>
       <c r="I37" s="3">
@@ -2740,7 +2740,7 @@
         <v>26.9</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.8000000000000007</v>
       </c>
       <c r="L37" s="3">
@@ -2779,7 +2779,7 @@
         <v>88</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.5999999999999943</v>
       </c>
       <c r="E38" s="3">
@@ -2792,7 +2792,7 @@
         <v>29.1</v>
       </c>
       <c r="H38" s="3">
-        <f>G38-F38</f>
+        <f t="shared" si="3"/>
         <v>-1.1999999999999993</v>
       </c>
       <c r="I38" s="3">
@@ -2802,7 +2802,7 @@
         <v>24.9</v>
       </c>
       <c r="K38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-15.600000000000001</v>
       </c>
       <c r="L38" s="3">
@@ -2841,7 +2841,7 @@
         <v>83.3</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.40000000000000568</v>
       </c>
       <c r="E39" s="5">
@@ -2854,7 +2854,7 @@
         <v>26.3</v>
       </c>
       <c r="H39" s="3">
-        <f>G39-F39</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="I39" s="3">
@@ -2864,7 +2864,7 @@
         <v>26.2</v>
       </c>
       <c r="K39" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.59999999999999787</v>
       </c>
       <c r="L39" s="3">
@@ -2903,7 +2903,7 @@
         <v>88.5</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.90000000000000568</v>
       </c>
       <c r="E40" s="3">
@@ -2916,7 +2916,7 @@
         <v>26.1</v>
       </c>
       <c r="H40" s="3">
-        <f>G40-F40</f>
+        <f t="shared" si="3"/>
         <v>-9.9999999999997868E-2</v>
       </c>
       <c r="I40" s="3">
@@ -2926,7 +2926,7 @@
         <v>25.1</v>
       </c>
       <c r="K40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="L40" s="3">
@@ -2965,7 +2965,7 @@
         <v>80.400000000000006</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="E41" s="3">
@@ -2978,7 +2978,7 @@
         <v>26.3</v>
       </c>
       <c r="H41" s="3">
-        <f>G41-F41</f>
+        <f t="shared" si="3"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="I41" s="3">
@@ -2988,7 +2988,7 @@
         <v>15.5</v>
       </c>
       <c r="K41" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.1000000000000014</v>
       </c>
       <c r="L41" s="3">
@@ -3027,7 +3027,7 @@
         <v>94.4</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.39999999999999147</v>
       </c>
       <c r="E42" s="3">
@@ -3040,7 +3040,7 @@
         <v>28.2</v>
       </c>
       <c r="H42" s="3">
-        <f>G42-F42</f>
+        <f t="shared" si="3"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="I42" s="3">
@@ -3050,7 +3050,7 @@
         <v>26.5</v>
       </c>
       <c r="K42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6000000000000014</v>
       </c>
       <c r="L42" s="3">
@@ -3089,7 +3089,7 @@
         <v>103.4</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.29999999999999716</v>
       </c>
       <c r="E43" s="3">
@@ -3102,7 +3102,7 @@
         <v>29.9</v>
       </c>
       <c r="H43" s="3">
-        <f>G43-F43</f>
+        <f t="shared" si="3"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="I43" s="3">
@@ -3112,7 +3112,7 @@
         <v>24.7</v>
       </c>
       <c r="K43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.3000000000000007</v>
       </c>
       <c r="L43" s="3">
@@ -3151,7 +3151,7 @@
         <v>94.2</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.7000000000000028</v>
       </c>
       <c r="E44" s="3">
@@ -3164,7 +3164,7 @@
         <v>32.6</v>
       </c>
       <c r="H44" s="3">
-        <f>G44-F44</f>
+        <f t="shared" si="3"/>
         <v>-0.60000000000000142</v>
       </c>
       <c r="I44" s="3">
@@ -3174,7 +3174,7 @@
         <v>31.8</v>
       </c>
       <c r="K44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.0999999999999979</v>
       </c>
       <c r="L44" s="3">
@@ -3213,7 +3213,7 @@
         <v>91.1</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.2000000000000028</v>
       </c>
       <c r="E45" s="3">
@@ -3226,7 +3226,7 @@
         <v>29.7</v>
       </c>
       <c r="H45" s="3">
-        <f>G45-F45</f>
+        <f t="shared" si="3"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="I45" s="3">
@@ -3236,7 +3236,7 @@
         <v>29.1</v>
       </c>
       <c r="K45" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.59999999999999787</v>
       </c>
       <c r="L45" s="3">
@@ -3275,7 +3275,7 @@
         <v>76.8</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.29999999999999716</v>
       </c>
       <c r="E46" s="3">
@@ -3288,7 +3288,7 @@
         <v>26.3</v>
       </c>
       <c r="H46" s="3">
-        <f>G46-F46</f>
+        <f t="shared" si="3"/>
         <v>6.1999999999999993</v>
       </c>
       <c r="I46" s="3">
@@ -3298,7 +3298,7 @@
         <v>19.8</v>
       </c>
       <c r="K46" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.5</v>
       </c>
       <c r="L46" s="3">
@@ -3337,7 +3337,7 @@
         <v>85.2</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="E47" s="3">
@@ -3350,7 +3350,7 @@
         <v>31.7</v>
       </c>
       <c r="H47" s="3">
-        <f>G47-F47</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="I47" s="3">
@@ -3360,7 +3360,7 @@
         <v>29.4</v>
       </c>
       <c r="K47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="L47" s="3">
@@ -3399,7 +3399,7 @@
         <v>65.8</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.60000000000000853</v>
       </c>
       <c r="E48" s="3">
@@ -3412,7 +3412,7 @@
         <v>28.5</v>
       </c>
       <c r="H48" s="3">
-        <f>G48-F48</f>
+        <f t="shared" si="3"/>
         <v>-0.19999999999999929</v>
       </c>
       <c r="I48" s="3">
@@ -3422,7 +3422,7 @@
         <v>41</v>
       </c>
       <c r="K48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2000000000000028</v>
       </c>
       <c r="L48" s="3">
@@ -3461,7 +3461,7 @@
         <v>77</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5999999999999943</v>
       </c>
       <c r="E49" s="3">
@@ -3474,7 +3474,7 @@
         <v>27.6</v>
       </c>
       <c r="H49" s="3">
-        <f>G49-F49</f>
+        <f t="shared" si="3"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I49" s="3">
@@ -3484,7 +3484,7 @@
         <v>38.700000000000003</v>
       </c>
       <c r="K49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.0999999999999943</v>
       </c>
       <c r="L49" s="3">
@@ -3523,7 +3523,7 @@
         <v>71.8</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8999999999999915</v>
       </c>
       <c r="E50" s="3">
@@ -3536,7 +3536,7 @@
         <v>28</v>
       </c>
       <c r="H50" s="3">
-        <f>G50-F50</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I50" s="3">
@@ -3546,7 +3546,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="K50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3999999999999986</v>
       </c>
       <c r="L50" s="3">
@@ -3585,7 +3585,7 @@
         <v>71.2</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2999999999999972</v>
       </c>
       <c r="E51" s="3">
@@ -3598,7 +3598,7 @@
         <v>28.2</v>
       </c>
       <c r="H51" s="3">
-        <f>G51-F51</f>
+        <f t="shared" si="3"/>
         <v>2.5999999999999979</v>
       </c>
       <c r="I51" s="3">
@@ -3608,7 +3608,7 @@
         <v>37</v>
       </c>
       <c r="K51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.2</v>
       </c>
       <c r="L51" s="3">
@@ -3647,7 +3647,7 @@
         <v>74.2</v>
       </c>
       <c r="D52" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.60000000000000853</v>
       </c>
       <c r="E52" s="3">
@@ -3660,7 +3660,7 @@
         <v>25.6</v>
       </c>
       <c r="H52" s="3">
-        <f>G52-F52</f>
+        <f t="shared" si="3"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="I52" s="3">
@@ -3670,7 +3670,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="K52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.39999999999999858</v>
       </c>
       <c r="L52" s="3">
@@ -3709,7 +3709,7 @@
         <v>82</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E53" s="3">
@@ -3722,7 +3722,7 @@
         <v>30.1</v>
       </c>
       <c r="H53" s="3">
-        <f>G53-F53</f>
+        <f t="shared" si="3"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="I53" s="3">
@@ -3732,7 +3732,7 @@
         <v>39.799999999999997</v>
       </c>
       <c r="K53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="L53" s="3">
@@ -3769,7 +3769,7 @@
         <v>80.3</v>
       </c>
       <c r="D54" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="E54" s="3">
@@ -3782,7 +3782,7 @@
         <v>30.2</v>
       </c>
       <c r="H54" s="3">
-        <f>G54-F54</f>
+        <f t="shared" si="3"/>
         <v>0.80000000000000071</v>
       </c>
       <c r="I54" s="3">
@@ -3792,7 +3792,7 @@
         <v>43.2</v>
       </c>
       <c r="K54" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.2000000000000028</v>
       </c>
       <c r="L54" s="3">
@@ -3831,7 +3831,7 @@
         <v>73.8</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E55" s="3">
@@ -3844,7 +3844,7 @@
         <v>29.2</v>
       </c>
       <c r="H55" s="3">
-        <f>G55-F55</f>
+        <f t="shared" si="3"/>
         <v>1.0999999999999979</v>
       </c>
       <c r="I55" s="3">
@@ -3854,7 +3854,7 @@
         <v>40.4</v>
       </c>
       <c r="K55" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6000000000000014</v>
       </c>
       <c r="L55" s="3">
@@ -3893,7 +3893,7 @@
         <v>71.900000000000006</v>
       </c>
       <c r="D56" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="E56" s="3">
@@ -3906,7 +3906,7 @@
         <v>27.4</v>
       </c>
       <c r="H56" s="3">
-        <f>G56-F56</f>
+        <f t="shared" si="3"/>
         <v>-0.40000000000000213</v>
       </c>
       <c r="I56" s="3">
@@ -3916,7 +3916,7 @@
         <v>39.299999999999997</v>
       </c>
       <c r="K56" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.1000000000000014</v>
       </c>
       <c r="L56" s="3">
@@ -3955,7 +3955,7 @@
         <v>89.1</v>
       </c>
       <c r="D57" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6999999999999886</v>
       </c>
       <c r="E57" s="3">
@@ -3968,7 +3968,7 @@
         <v>32.700000000000003</v>
       </c>
       <c r="H57" s="3">
-        <f>G57-F57</f>
+        <f t="shared" si="3"/>
         <v>1.0000000000000036</v>
       </c>
       <c r="I57" s="3">
@@ -3978,7 +3978,7 @@
         <v>42.6</v>
       </c>
       <c r="K57" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="L57" s="3">
@@ -4017,7 +4017,7 @@
         <v>68.599999999999994</v>
       </c>
       <c r="D58" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="E58" s="3">
@@ -4030,7 +4030,7 @@
         <v>29.3</v>
       </c>
       <c r="H58" s="3">
-        <f>G58-F58</f>
+        <f t="shared" si="3"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="I58" s="3">
@@ -4040,7 +4040,7 @@
         <v>40.799999999999997</v>
       </c>
       <c r="K58" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.399999999999999</v>
       </c>
       <c r="L58" s="3">
@@ -4079,7 +4079,7 @@
         <v>71.5</v>
       </c>
       <c r="D59" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.9999999999994316E-2</v>
       </c>
       <c r="E59" s="3">
@@ -4092,7 +4092,7 @@
         <v>26.2</v>
       </c>
       <c r="H59" s="3">
-        <f>G59-F59</f>
+        <f t="shared" si="3"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="I59" s="3">
@@ -4102,7 +4102,7 @@
         <v>31.6</v>
       </c>
       <c r="K59" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.1999999999999957</v>
       </c>
       <c r="L59" s="3">
@@ -4141,7 +4141,7 @@
         <v>81.3</v>
       </c>
       <c r="D60" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E60" s="3">
@@ -4154,7 +4154,7 @@
         <v>25.7</v>
       </c>
       <c r="H60" s="3">
-        <f>G60-F60</f>
+        <f t="shared" si="3"/>
         <v>0.39999999999999858</v>
       </c>
       <c r="I60" s="3">
@@ -4164,7 +4164,7 @@
         <v>27.2</v>
       </c>
       <c r="K60" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="L60" s="3">
@@ -4203,7 +4203,7 @@
         <v>85.2</v>
       </c>
       <c r="D61" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.29999999999999716</v>
       </c>
       <c r="E61" s="3">
@@ -4216,7 +4216,7 @@
         <v>27.8</v>
       </c>
       <c r="H61" s="3">
-        <f>G61-F61</f>
+        <f t="shared" si="3"/>
         <v>-9.9999999999997868E-2</v>
       </c>
       <c r="I61" s="3">
@@ -4226,7 +4226,7 @@
         <v>42.4</v>
       </c>
       <c r="K61" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="L61" s="3">
@@ -4265,7 +4265,7 @@
         <v>77.900000000000006</v>
       </c>
       <c r="D62" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.40000000000000568</v>
       </c>
       <c r="E62" s="3">
@@ -4278,7 +4278,7 @@
         <v>26.6</v>
       </c>
       <c r="H62" s="3">
-        <f>G62-F62</f>
+        <f t="shared" si="3"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="I62" s="3">
@@ -4288,7 +4288,7 @@
         <v>35.799999999999997</v>
       </c>
       <c r="K62" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.3000000000000043</v>
       </c>
       <c r="L62" s="3">
@@ -4327,7 +4327,7 @@
         <v>87.5</v>
       </c>
       <c r="D63" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.29999999999999716</v>
       </c>
       <c r="E63" s="3">
@@ -4340,7 +4340,7 @@
         <v>27</v>
       </c>
       <c r="H63" s="3">
-        <f>G63-F63</f>
+        <f t="shared" si="3"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="I63" s="3">
@@ -4350,7 +4350,7 @@
         <v>42.9</v>
       </c>
       <c r="K63" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.30000000000000426</v>
       </c>
       <c r="L63" s="3">
@@ -4389,7 +4389,7 @@
         <v>81.599999999999994</v>
       </c>
       <c r="D64" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.9000000000000057</v>
       </c>
       <c r="E64" s="3">
@@ -4402,7 +4402,7 @@
         <v>31.8</v>
       </c>
       <c r="H64" s="3">
-        <f>G64-F64</f>
+        <f t="shared" si="3"/>
         <v>-2.0999999999999979</v>
       </c>
       <c r="I64" s="3">
@@ -4412,7 +4412,7 @@
         <v>39.4</v>
       </c>
       <c r="K64" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2999999999999972</v>
       </c>
       <c r="L64" s="3">
@@ -4451,7 +4451,7 @@
         <v>90.2</v>
       </c>
       <c r="D65" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.9999999999994316E-2</v>
       </c>
       <c r="E65" s="3">
@@ -4464,7 +4464,7 @@
         <v>30.8</v>
       </c>
       <c r="H65" s="3">
-        <f>G65-F65</f>
+        <f t="shared" si="3"/>
         <v>-9.9999999999997868E-2</v>
       </c>
       <c r="I65" s="3">
@@ -4474,7 +4474,7 @@
         <v>29.6</v>
       </c>
       <c r="K65" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.7999999999999972</v>
       </c>
       <c r="L65" s="3">
@@ -4511,7 +4511,7 @@
         <v>79.2</v>
       </c>
       <c r="D66" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.60000000000000853</v>
       </c>
       <c r="E66" s="3">
@@ -4524,7 +4524,7 @@
         <v>28.1</v>
       </c>
       <c r="H66" s="3">
-        <f>G66-F66</f>
+        <f t="shared" ref="H66:H97" si="4">G66-F66</f>
         <v>0.30000000000000071</v>
       </c>
       <c r="I66" s="3">
@@ -4534,7 +4534,7 @@
         <v>41.5</v>
       </c>
       <c r="K66" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="L66" s="3">
@@ -4571,7 +4571,7 @@
         <v>104.6</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" ref="D67:D130" si="2">C67-B67</f>
+        <f t="shared" ref="D67:D130" si="5">C67-B67</f>
         <v>-0.90000000000000568</v>
       </c>
       <c r="E67" s="3">
@@ -4584,7 +4584,7 @@
         <v>28.4</v>
       </c>
       <c r="H67" s="3">
-        <f>G67-F67</f>
+        <f t="shared" si="4"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="I67" s="3">
@@ -4594,7 +4594,7 @@
         <v>23.3</v>
       </c>
       <c r="K67" s="3">
-        <f t="shared" ref="K67:K130" si="3">J67-I67</f>
+        <f t="shared" ref="K67:K130" si="6">J67-I67</f>
         <v>-0.80000000000000071</v>
       </c>
       <c r="L67" s="3">
@@ -4633,7 +4633,7 @@
         <v>86.5</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.9999999999994316E-2</v>
       </c>
       <c r="E68" s="3">
@@ -4646,7 +4646,7 @@
         <v>28.9</v>
       </c>
       <c r="H68" s="3">
-        <f>G68-F68</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I68" s="3">
@@ -4656,7 +4656,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="K68" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-5.7999999999999972</v>
       </c>
       <c r="L68" s="3">
@@ -4695,7 +4695,7 @@
         <v>89.7</v>
       </c>
       <c r="D69" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.2999999999999972</v>
       </c>
       <c r="E69" s="3">
@@ -4708,7 +4708,7 @@
         <v>26.8</v>
       </c>
       <c r="H69" s="3">
-        <f>G69-F69</f>
+        <f t="shared" si="4"/>
         <v>-0.69999999999999929</v>
       </c>
       <c r="I69" s="3">
@@ -4718,7 +4718,7 @@
         <v>14.4</v>
       </c>
       <c r="K69" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-3.4999999999999982</v>
       </c>
       <c r="L69" s="3">
@@ -4757,7 +4757,7 @@
         <v>70</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.0999999999999943</v>
       </c>
       <c r="E70" s="3">
@@ -4770,7 +4770,7 @@
         <v>28</v>
       </c>
       <c r="H70" s="3">
-        <f>G70-F70</f>
+        <f t="shared" si="4"/>
         <v>0.69999999999999929</v>
       </c>
       <c r="I70" s="3">
@@ -4780,7 +4780,7 @@
         <v>40.700000000000003</v>
       </c>
       <c r="K70" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.2000000000000028</v>
       </c>
       <c r="L70" s="3">
@@ -4817,7 +4817,7 @@
         <v>80.400000000000006</v>
       </c>
       <c r="D71" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.5</v>
       </c>
       <c r="E71" s="3">
@@ -4830,7 +4830,7 @@
         <v>27.2</v>
       </c>
       <c r="H71" s="3">
-        <f>G71-F71</f>
+        <f t="shared" si="4"/>
         <v>-0.80000000000000071</v>
       </c>
       <c r="I71" s="3">
@@ -4840,7 +4840,7 @@
         <v>30.6</v>
       </c>
       <c r="K71" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="L71" s="3">
@@ -4879,7 +4879,7 @@
         <v>73</v>
       </c>
       <c r="D72" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2</v>
       </c>
       <c r="E72" s="3">
@@ -4892,7 +4892,7 @@
         <v>25.6</v>
       </c>
       <c r="H72" s="3">
-        <f>G72-F72</f>
+        <f t="shared" si="4"/>
         <v>-0.69999999999999929</v>
       </c>
       <c r="I72" s="3">
@@ -4902,7 +4902,7 @@
         <v>25.9</v>
       </c>
       <c r="K72" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2</v>
       </c>
       <c r="L72" s="3">
@@ -4941,7 +4941,7 @@
         <v>80.900000000000006</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.6999999999999886</v>
       </c>
       <c r="E73" s="3">
@@ -4954,7 +4954,7 @@
         <v>26.7</v>
       </c>
       <c r="H73" s="3">
-        <f>G73-F73</f>
+        <f t="shared" si="4"/>
         <v>-0.30000000000000071</v>
       </c>
       <c r="I73" s="3">
@@ -4964,7 +4964,7 @@
         <v>21.2</v>
       </c>
       <c r="K73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L73" s="3">
@@ -5003,7 +5003,7 @@
         <v>83.9</v>
       </c>
       <c r="D74" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.29999999999999716</v>
       </c>
       <c r="E74" s="3">
@@ -5016,7 +5016,7 @@
         <v>28.3</v>
       </c>
       <c r="H74" s="3">
-        <f>G74-F74</f>
+        <f t="shared" si="4"/>
         <v>-0.19999999999999929</v>
       </c>
       <c r="I74" s="3">
@@ -5026,7 +5026,7 @@
         <v>26.9</v>
       </c>
       <c r="K74" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-8.3000000000000043</v>
       </c>
       <c r="L74" s="3">
@@ -5065,7 +5065,7 @@
         <v>88.6</v>
       </c>
       <c r="D75" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.89999999999999147</v>
       </c>
       <c r="E75" s="3">
@@ -5078,7 +5078,7 @@
         <v>27.7</v>
       </c>
       <c r="H75" s="3">
-        <f>G75-F75</f>
+        <f t="shared" si="4"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="I75" s="3">
@@ -5088,7 +5088,7 @@
         <v>26.4</v>
       </c>
       <c r="K75" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.3999999999999986</v>
       </c>
       <c r="L75" s="3">
@@ -5127,7 +5127,7 @@
         <v>84.5</v>
       </c>
       <c r="D76" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.59999999999999432</v>
       </c>
       <c r="E76" s="3">
@@ -5140,7 +5140,7 @@
         <v>26.4</v>
       </c>
       <c r="H76" s="3">
-        <f>G76-F76</f>
+        <f t="shared" si="4"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I76" s="3">
@@ -5150,7 +5150,7 @@
         <v>21.7</v>
       </c>
       <c r="K76" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="L76" s="3">
@@ -5189,7 +5189,7 @@
         <v>96.4</v>
       </c>
       <c r="D77" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="E77" s="3">
@@ -5202,7 +5202,7 @@
         <v>30.1</v>
       </c>
       <c r="H77" s="3">
-        <f>G77-F77</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="I77" s="3">
@@ -5212,7 +5212,7 @@
         <v>30.8</v>
       </c>
       <c r="K77" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.9999999999999964</v>
       </c>
       <c r="L77" s="3">
@@ -5251,7 +5251,7 @@
         <v>72.599999999999994</v>
       </c>
       <c r="D78" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="E78" s="3">
@@ -5264,7 +5264,7 @@
         <v>27</v>
       </c>
       <c r="H78" s="3">
-        <f>G78-F78</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="I78" s="3">
@@ -5274,7 +5274,7 @@
         <v>26.4</v>
       </c>
       <c r="K78" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.2999999999999972</v>
       </c>
       <c r="L78" s="3">
@@ -5313,7 +5313,7 @@
         <v>91.9</v>
       </c>
       <c r="D79" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.9000000000000057</v>
       </c>
       <c r="E79" s="3">
@@ -5326,7 +5326,7 @@
         <v>30</v>
       </c>
       <c r="H79" s="3">
-        <f>G79-F79</f>
+        <f t="shared" si="4"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I79" s="8"/>
@@ -5368,7 +5368,7 @@
         <v>75.599999999999994</v>
       </c>
       <c r="D80" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.79999999999999716</v>
       </c>
       <c r="E80" s="3">
@@ -5381,7 +5381,7 @@
         <v>27.7</v>
       </c>
       <c r="H80" s="3">
-        <f>G80-F80</f>
+        <f t="shared" si="4"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I80" s="3">
@@ -5391,7 +5391,7 @@
         <v>19.899999999999999</v>
       </c>
       <c r="K80" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="L80" s="3">
@@ -5430,7 +5430,7 @@
         <v>81.8</v>
       </c>
       <c r="D81" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="E81" s="3">
@@ -5443,7 +5443,7 @@
         <v>25.2</v>
       </c>
       <c r="H81" s="3">
-        <f>G81-F81</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I81" s="3">
@@ -5453,7 +5453,7 @@
         <v>22.5</v>
       </c>
       <c r="K81" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.69999999999999929</v>
       </c>
       <c r="L81" s="3">
@@ -5492,7 +5492,7 @@
         <v>94.5</v>
       </c>
       <c r="D82" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="E82" s="3">
@@ -5505,7 +5505,7 @@
         <v>27.9</v>
       </c>
       <c r="H82" s="3">
-        <f>G82-F82</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I82" s="3">
@@ -5515,7 +5515,7 @@
         <v>26.3</v>
       </c>
       <c r="K82" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.5999999999999979</v>
       </c>
       <c r="L82" s="3">
@@ -5554,7 +5554,7 @@
         <v>79.2</v>
       </c>
       <c r="D83" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.90000000000000568</v>
       </c>
       <c r="E83" s="3">
@@ -5567,7 +5567,7 @@
         <v>24.7</v>
       </c>
       <c r="H83" s="3">
-        <f>G83-F83</f>
+        <f t="shared" si="4"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="I83" s="3">
@@ -5577,7 +5577,7 @@
         <v>25.8</v>
       </c>
       <c r="K83" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4000000000000021</v>
       </c>
       <c r="L83" s="3">
@@ -5616,7 +5616,7 @@
         <v>81.599999999999994</v>
       </c>
       <c r="D84" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.10000000000000853</v>
       </c>
       <c r="E84" s="3">
@@ -5629,7 +5629,7 @@
         <v>25.1</v>
       </c>
       <c r="H84" s="3">
-        <f>G84-F84</f>
+        <f t="shared" si="4"/>
         <v>-9.9999999999997868E-2</v>
       </c>
       <c r="I84" s="3">
@@ -5639,7 +5639,7 @@
         <v>21.9</v>
       </c>
       <c r="K84" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.2000000000000028</v>
       </c>
       <c r="L84" s="3">
@@ -5678,7 +5678,7 @@
         <v>106.8</v>
       </c>
       <c r="D85" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.79999999999999716</v>
       </c>
       <c r="E85" s="3">
@@ -5691,7 +5691,7 @@
         <v>31.9</v>
       </c>
       <c r="H85" s="3">
-        <f>G85-F85</f>
+        <f t="shared" si="4"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I85" s="3">
@@ -5701,7 +5701,7 @@
         <v>32.700000000000003</v>
       </c>
       <c r="K85" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.59999999999999432</v>
       </c>
       <c r="L85" s="3">
@@ -5740,7 +5740,7 @@
         <v>78.400000000000006</v>
       </c>
       <c r="D86" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.8000000000000114</v>
       </c>
       <c r="E86" s="3">
@@ -5753,7 +5753,7 @@
         <v>26.2</v>
       </c>
       <c r="H86" s="3">
-        <f>G86-F86</f>
+        <f t="shared" si="4"/>
         <v>0.59999999999999787</v>
       </c>
       <c r="I86" s="3">
@@ -5763,7 +5763,7 @@
         <v>18</v>
       </c>
       <c r="K86" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-4.8000000000000007</v>
       </c>
       <c r="L86" s="3">
@@ -5802,7 +5802,7 @@
         <v>79.8</v>
       </c>
       <c r="D87" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="E87" s="3">
@@ -5815,7 +5815,7 @@
         <v>24.4</v>
       </c>
       <c r="H87" s="3">
-        <f>G87-F87</f>
+        <f t="shared" si="4"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I87" s="3">
@@ -5825,7 +5825,7 @@
         <v>23.5</v>
       </c>
       <c r="K87" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.6000000000000014</v>
       </c>
       <c r="L87" s="3">
@@ -5864,7 +5864,7 @@
         <v>98.7</v>
       </c>
       <c r="D88" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.90000000000000568</v>
       </c>
       <c r="E88" s="3">
@@ -5877,7 +5877,7 @@
         <v>27.3</v>
       </c>
       <c r="H88" s="3">
-        <f>G88-F88</f>
+        <f t="shared" si="4"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I88" s="3">
@@ -5887,7 +5887,7 @@
         <v>29</v>
       </c>
       <c r="K88" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="L88" s="3">
@@ -5926,7 +5926,7 @@
         <v>93.5</v>
       </c>
       <c r="D89" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E89" s="3">
@@ -5939,7 +5939,7 @@
         <v>30.5</v>
       </c>
       <c r="H89" s="3">
-        <f>G89-F89</f>
+        <f t="shared" si="4"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I89" s="3">
@@ -5949,7 +5949,7 @@
         <v>27.9</v>
       </c>
       <c r="K89" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.5999999999999979</v>
       </c>
       <c r="L89" s="3">
@@ -5988,7 +5988,7 @@
         <v>69.400000000000006</v>
       </c>
       <c r="D90" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="E90" s="3">
@@ -6001,7 +6001,7 @@
         <v>24.6</v>
       </c>
       <c r="H90" s="3">
-        <f>G90-F90</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="I90" s="3">
@@ -6011,7 +6011,7 @@
         <v>24.9</v>
       </c>
       <c r="K90" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="L90" s="3">
@@ -6050,7 +6050,7 @@
         <v>85.2</v>
       </c>
       <c r="D91" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.6000000000000085</v>
       </c>
       <c r="E91" s="3">
@@ -6063,7 +6063,7 @@
         <v>25.7</v>
       </c>
       <c r="H91" s="3">
-        <f>G91-F91</f>
+        <f t="shared" si="4"/>
         <v>-0.40000000000000213</v>
       </c>
       <c r="I91" s="3">
@@ -6073,7 +6073,7 @@
         <v>22.6</v>
       </c>
       <c r="K91" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-3</v>
       </c>
       <c r="L91" s="3">
@@ -6112,7 +6112,7 @@
         <v>116.8</v>
       </c>
       <c r="D92" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="E92" s="3">
@@ -6125,7 +6125,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="H92" s="3">
-        <f>G92-F92</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I92" s="3">
@@ -6135,7 +6135,7 @@
         <v>33.299999999999997</v>
       </c>
       <c r="K92" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-4</v>
       </c>
       <c r="L92" s="3">
@@ -6174,7 +6174,7 @@
         <v>77.5</v>
       </c>
       <c r="D93" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.7000000000000028</v>
       </c>
       <c r="E93" s="3">
@@ -6187,7 +6187,7 @@
         <v>25.9</v>
       </c>
       <c r="H93" s="3">
-        <f>G93-F93</f>
+        <f t="shared" si="4"/>
         <v>0.59999999999999787</v>
       </c>
       <c r="I93" s="3">
@@ -6197,7 +6197,7 @@
         <v>24.8</v>
       </c>
       <c r="K93" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-11.400000000000002</v>
       </c>
       <c r="L93" s="3">
@@ -6236,7 +6236,7 @@
         <v>79.900000000000006</v>
       </c>
       <c r="D94" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.4000000000000057</v>
       </c>
       <c r="E94" s="3">
@@ -6249,7 +6249,7 @@
         <v>28.7</v>
       </c>
       <c r="H94" s="3">
-        <f>G94-F94</f>
+        <f t="shared" si="4"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="I94" s="3">
@@ -6259,7 +6259,7 @@
         <v>41.4</v>
       </c>
       <c r="K94" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="L94" s="3">
@@ -6298,7 +6298,7 @@
         <v>83</v>
       </c>
       <c r="D95" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="E95" s="3">
@@ -6311,7 +6311,7 @@
         <v>31.6</v>
       </c>
       <c r="H95" s="3">
-        <f>G95-F95</f>
+        <f t="shared" si="4"/>
         <v>-0.39999999999999858</v>
       </c>
       <c r="I95" s="3">
@@ -6321,7 +6321,7 @@
         <v>42.9</v>
       </c>
       <c r="K95" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L95" s="3">
@@ -6360,7 +6360,7 @@
         <v>58</v>
       </c>
       <c r="D96" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="E96" s="3">
@@ -6373,7 +6373,7 @@
         <v>25.1</v>
       </c>
       <c r="H96" s="3">
-        <f>G96-F96</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I96" s="3">
@@ -6383,7 +6383,7 @@
         <v>31</v>
       </c>
       <c r="K96" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="L96" s="3">
@@ -6422,7 +6422,7 @@
         <v>95.2</v>
       </c>
       <c r="D97" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="E97" s="3">
@@ -6435,7 +6435,7 @@
         <v>32.9</v>
       </c>
       <c r="H97" s="3">
-        <f>G97-F97</f>
+        <f t="shared" si="4"/>
         <v>0.39999999999999858</v>
       </c>
       <c r="I97" s="3">
@@ -6445,7 +6445,7 @@
         <v>44.9</v>
       </c>
       <c r="K97" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.1000000000000014</v>
       </c>
       <c r="L97" s="3">
@@ -6484,7 +6484,7 @@
         <v>73.2</v>
       </c>
       <c r="D98" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.4000000000000057</v>
       </c>
       <c r="E98" s="3">
@@ -6497,7 +6497,7 @@
         <v>27.3</v>
       </c>
       <c r="H98" s="3">
-        <f>G98-F98</f>
+        <f t="shared" ref="H98:H129" si="7">G98-F98</f>
         <v>1</v>
       </c>
       <c r="I98" s="3">
@@ -6507,7 +6507,7 @@
         <v>40.1</v>
       </c>
       <c r="K98" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.1000000000000014</v>
       </c>
       <c r="L98" s="3">
@@ -6546,7 +6546,7 @@
         <v>65.599999999999994</v>
       </c>
       <c r="D99" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.79999999999999716</v>
       </c>
       <c r="E99" s="3">
@@ -6559,7 +6559,7 @@
         <v>26.6</v>
       </c>
       <c r="H99" s="3">
-        <f>G99-F99</f>
+        <f t="shared" si="7"/>
         <v>-1.5</v>
       </c>
       <c r="I99" s="3">
@@ -6569,7 +6569,7 @@
         <v>33.1</v>
       </c>
       <c r="K99" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.1000000000000014</v>
       </c>
       <c r="L99" s="3">
@@ -6608,7 +6608,7 @@
         <v>80.7</v>
       </c>
       <c r="D100" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.60000000000000853</v>
       </c>
       <c r="E100" s="3">
@@ -6621,7 +6621,7 @@
         <v>29.3</v>
       </c>
       <c r="H100" s="3">
-        <f>G100-F100</f>
+        <f t="shared" si="7"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I100" s="3">
@@ -6631,7 +6631,7 @@
         <v>38.9</v>
       </c>
       <c r="K100" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.89999999999999858</v>
       </c>
       <c r="L100" s="3">
@@ -6670,7 +6670,7 @@
         <v>93.3</v>
       </c>
       <c r="D101" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.59999999999999432</v>
       </c>
       <c r="E101" s="3">
@@ -6683,7 +6683,7 @@
         <v>33.5</v>
       </c>
       <c r="H101" s="3">
-        <f>G101-F101</f>
+        <f t="shared" si="7"/>
         <v>-0.5</v>
       </c>
       <c r="I101" s="3">
@@ -6693,7 +6693,7 @@
         <v>47.5</v>
       </c>
       <c r="K101" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.7999999999999972</v>
       </c>
       <c r="L101" s="3">
@@ -6732,7 +6732,7 @@
         <v>86.7</v>
       </c>
       <c r="D102" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E102" s="3">
@@ -6745,7 +6745,7 @@
         <v>31.1</v>
       </c>
       <c r="H102" s="3">
-        <f>G102-F102</f>
+        <f t="shared" si="7"/>
         <v>-0.39999999999999858</v>
       </c>
       <c r="I102" s="3">
@@ -6755,7 +6755,7 @@
         <v>43.4</v>
       </c>
       <c r="K102" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.3999999999999986</v>
       </c>
       <c r="L102" s="3">
@@ -6792,7 +6792,7 @@
         <v>66.900000000000006</v>
       </c>
       <c r="D103" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.6000000000000085</v>
       </c>
       <c r="E103" s="5">
@@ -6805,7 +6805,7 @@
         <v>25.5</v>
       </c>
       <c r="H103" s="3">
-        <f>G103-F103</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I103" s="3">
@@ -6815,7 +6815,7 @@
         <v>38.799999999999997</v>
       </c>
       <c r="K103" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="L103" s="3">
@@ -6854,7 +6854,7 @@
         <v>75.3</v>
       </c>
       <c r="D104" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="E104" s="3">
@@ -6867,7 +6867,7 @@
         <v>28</v>
       </c>
       <c r="H104" s="3">
-        <f>G104-F104</f>
+        <f t="shared" si="7"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I104" s="3">
@@ -6877,7 +6877,7 @@
         <v>40.200000000000003</v>
       </c>
       <c r="K104" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.2000000000000028</v>
       </c>
       <c r="L104" s="3">
@@ -6910,7 +6910,7 @@
         <v>83.7</v>
       </c>
       <c r="D105" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.2000000000000028</v>
       </c>
       <c r="E105" s="3">
@@ -6923,7 +6923,7 @@
         <v>28</v>
       </c>
       <c r="H105" s="3">
-        <f>G105-F105</f>
+        <f t="shared" si="7"/>
         <v>0.10000000000000142</v>
       </c>
       <c r="I105" s="3">
@@ -6933,7 +6933,7 @@
         <v>36.4</v>
       </c>
       <c r="K105" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L105" s="3">
@@ -6972,7 +6972,7 @@
         <v>65.599999999999994</v>
       </c>
       <c r="D106" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.39999999999999147</v>
       </c>
       <c r="E106" s="3">
@@ -6985,7 +6985,7 @@
         <v>24.8</v>
       </c>
       <c r="H106" s="3">
-        <f>G106-F106</f>
+        <f t="shared" si="7"/>
         <v>-0.39999999999999858</v>
       </c>
       <c r="I106" s="3">
@@ -6995,7 +6995,7 @@
         <v>26.1</v>
       </c>
       <c r="K106" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-13.5</v>
       </c>
       <c r="L106" s="3">
@@ -7034,7 +7034,7 @@
         <v>90.8</v>
       </c>
       <c r="D107" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.8999999999999915</v>
       </c>
       <c r="E107" s="3">
@@ -7047,7 +7047,7 @@
         <v>35.5</v>
       </c>
       <c r="H107" s="3">
-        <f>G107-F107</f>
+        <f t="shared" si="7"/>
         <v>1.2000000000000028</v>
       </c>
       <c r="I107" s="3">
@@ -7057,7 +7057,7 @@
         <v>45.9</v>
       </c>
       <c r="K107" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="L107" s="3">
@@ -7096,7 +7096,7 @@
         <v>93.6</v>
       </c>
       <c r="D108" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.9000000000000057</v>
       </c>
       <c r="E108" s="3">
@@ -7109,7 +7109,7 @@
         <v>33.6</v>
       </c>
       <c r="H108" s="3">
-        <f>G108-F108</f>
+        <f t="shared" si="7"/>
         <v>-1.2999999999999972</v>
       </c>
       <c r="I108" s="3">
@@ -7119,7 +7119,7 @@
         <v>43</v>
       </c>
       <c r="K108" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-5.7000000000000028</v>
       </c>
       <c r="L108" s="3">
@@ -7158,7 +7158,7 @@
         <v>79.900000000000006</v>
       </c>
       <c r="D109" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.10000000000000853</v>
       </c>
       <c r="E109" s="3">
@@ -7171,7 +7171,7 @@
         <v>30.4</v>
       </c>
       <c r="H109" s="3">
-        <f>G109-F109</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I109" s="3">
@@ -7181,7 +7181,7 @@
         <v>39.6</v>
       </c>
       <c r="K109" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.3999999999999986</v>
       </c>
       <c r="L109" s="3">
@@ -7218,7 +7218,7 @@
         <v>79.8</v>
       </c>
       <c r="D110" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.39999999999999147</v>
       </c>
       <c r="E110" s="3">
@@ -7231,7 +7231,7 @@
         <v>32.4</v>
       </c>
       <c r="H110" s="3">
-        <f>G110-F110</f>
+        <f t="shared" si="7"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="I110" s="3">
@@ -7241,7 +7241,7 @@
         <v>42.2</v>
       </c>
       <c r="K110" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.5</v>
       </c>
       <c r="L110" s="3">
@@ -7280,7 +7280,7 @@
         <v>75.2</v>
       </c>
       <c r="D111" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.79999999999999716</v>
       </c>
       <c r="E111" s="3">
@@ -7293,7 +7293,7 @@
         <v>27.3</v>
       </c>
       <c r="H111" s="3">
-        <f>G111-F111</f>
+        <f t="shared" si="7"/>
         <v>0.30000000000000071</v>
       </c>
       <c r="I111" s="3">
@@ -7303,7 +7303,7 @@
         <v>41.5</v>
       </c>
       <c r="K111" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.3999999999999986</v>
       </c>
       <c r="L111" s="3">
@@ -7340,7 +7340,7 @@
         <v>101.1</v>
       </c>
       <c r="D112" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.0999999999999943</v>
       </c>
       <c r="E112" s="3">
@@ -7353,7 +7353,7 @@
         <v>30.2</v>
       </c>
       <c r="H112" s="3">
-        <f>G112-F112</f>
+        <f t="shared" si="7"/>
         <v>1.5999999999999979</v>
       </c>
       <c r="I112" s="3">
@@ -7363,7 +7363,7 @@
         <v>30.9</v>
       </c>
       <c r="K112" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="L112" s="3">
@@ -7402,7 +7402,7 @@
         <v>75.8</v>
       </c>
       <c r="D113" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.4000000000000057</v>
       </c>
       <c r="E113" s="3">
@@ -7415,7 +7415,7 @@
         <v>27.5</v>
       </c>
       <c r="H113" s="3">
-        <f>G113-F113</f>
+        <f t="shared" si="7"/>
         <v>-0.89999999999999858</v>
       </c>
       <c r="I113" s="3">
@@ -7425,7 +7425,7 @@
         <v>28.1</v>
       </c>
       <c r="K113" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.2999999999999972</v>
       </c>
       <c r="L113" s="3">
@@ -7462,7 +7462,7 @@
         <v>81</v>
       </c>
       <c r="D114" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="E114" s="3">
@@ -7475,7 +7475,7 @@
         <v>28</v>
       </c>
       <c r="H114" s="3">
-        <f>G114-F114</f>
+        <f t="shared" si="7"/>
         <v>-0.39999999999999858</v>
       </c>
       <c r="I114" s="3">
@@ -7485,7 +7485,7 @@
         <v>25.4</v>
       </c>
       <c r="K114" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.8000000000000007</v>
       </c>
       <c r="L114" s="3">
@@ -7524,7 +7524,7 @@
         <v>68.599999999999994</v>
       </c>
       <c r="D115" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.3000000000000114</v>
       </c>
       <c r="E115" s="3">
@@ -7537,7 +7537,7 @@
         <v>25.8</v>
       </c>
       <c r="H115" s="3">
-        <f>G115-F115</f>
+        <f t="shared" si="7"/>
         <v>-0.5</v>
       </c>
       <c r="I115" s="3">
@@ -7547,7 +7547,7 @@
         <v>21.7</v>
       </c>
       <c r="K115" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.3000000000000007</v>
       </c>
       <c r="L115" s="3">
@@ -7586,7 +7586,7 @@
         <v>84.7</v>
       </c>
       <c r="D116" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.6000000000000085</v>
       </c>
       <c r="E116" s="3">
@@ -7599,7 +7599,7 @@
         <v>27.7</v>
       </c>
       <c r="H116" s="3">
-        <f>G116-F116</f>
+        <f t="shared" si="7"/>
         <v>0.59999999999999787</v>
       </c>
       <c r="I116" s="3">
@@ -7609,7 +7609,7 @@
         <v>27.5</v>
       </c>
       <c r="K116" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.3000000000000007</v>
       </c>
       <c r="L116" s="3">
@@ -7648,7 +7648,7 @@
         <v>74.8</v>
       </c>
       <c r="D117" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.9999999999994316E-2</v>
       </c>
       <c r="E117" s="3">
@@ -7661,7 +7661,7 @@
         <v>26.2</v>
       </c>
       <c r="H117" s="3">
-        <f>G117-F117</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I117" s="3">
@@ -7671,7 +7671,7 @@
         <v>19.7</v>
       </c>
       <c r="K117" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.90000000000000213</v>
       </c>
       <c r="L117" s="3">
@@ -7710,7 +7710,7 @@
         <v>81.900000000000006</v>
       </c>
       <c r="D118" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.4000000000000057</v>
       </c>
       <c r="E118" s="3">
@@ -7723,7 +7723,7 @@
         <v>33.4</v>
       </c>
       <c r="H118" s="3">
-        <f>G118-F118</f>
+        <f t="shared" si="7"/>
         <v>4.5</v>
       </c>
       <c r="I118" s="3">
@@ -7733,7 +7733,7 @@
         <v>25.9</v>
       </c>
       <c r="K118" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="L118" s="3">
@@ -7772,7 +7772,7 @@
         <v>76.8</v>
       </c>
       <c r="D119" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.29999999999999716</v>
       </c>
       <c r="E119" s="3">
@@ -7785,7 +7785,7 @@
         <v>26.3</v>
       </c>
       <c r="H119" s="3">
-        <f>G119-F119</f>
+        <f t="shared" si="7"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I119" s="3">
@@ -7795,7 +7795,7 @@
         <v>22.6</v>
       </c>
       <c r="K119" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.8999999999999986</v>
       </c>
       <c r="L119" s="3">
@@ -7834,7 +7834,7 @@
         <v>96.3</v>
       </c>
       <c r="D120" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.2999999999999972</v>
       </c>
       <c r="E120" s="3">
@@ -7847,7 +7847,7 @@
         <v>28.1</v>
       </c>
       <c r="H120" s="3">
-        <f>G120-F120</f>
+        <f t="shared" si="7"/>
         <v>0.40000000000000213</v>
       </c>
       <c r="I120" s="3">
@@ -7857,7 +7857,7 @@
         <v>24.7</v>
       </c>
       <c r="K120" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.6999999999999993</v>
       </c>
       <c r="L120" s="3">
@@ -7896,7 +7896,7 @@
         <v>78.2</v>
       </c>
       <c r="D121" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.39999999999999147</v>
       </c>
       <c r="E121" s="3">
@@ -7909,7 +7909,7 @@
         <v>24.4</v>
       </c>
       <c r="H121" s="3">
-        <f>G121-F121</f>
+        <f t="shared" si="7"/>
         <v>-0.10000000000000142</v>
       </c>
       <c r="I121" s="3">
@@ -7919,7 +7919,7 @@
         <v>19.5</v>
       </c>
       <c r="K121" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.3000000000000007</v>
       </c>
       <c r="L121" s="3">
@@ -7952,7 +7952,7 @@
         <v>76.7</v>
       </c>
       <c r="D122" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.3999999999999915</v>
       </c>
       <c r="E122" s="3">
@@ -7965,7 +7965,7 @@
         <v>26.5</v>
       </c>
       <c r="H122" s="3">
-        <f>G122-F122</f>
+        <f t="shared" si="7"/>
         <v>-0.89999999999999858</v>
       </c>
       <c r="I122" s="3">
@@ -7975,7 +7975,7 @@
         <v>15.1</v>
       </c>
       <c r="K122" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.9000000000000004</v>
       </c>
       <c r="L122" s="3">
@@ -8014,7 +8014,7 @@
         <v>76.7</v>
       </c>
       <c r="D123" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.79999999999999716</v>
       </c>
       <c r="E123" s="3">
@@ -8027,7 +8027,7 @@
         <v>24.5</v>
       </c>
       <c r="H123" s="3">
-        <f>G123-F123</f>
+        <f t="shared" si="7"/>
         <v>-0.30000000000000071</v>
       </c>
       <c r="I123" s="3">
@@ -8037,7 +8037,7 @@
         <v>15</v>
       </c>
       <c r="K123" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.5</v>
       </c>
       <c r="L123" s="3">
@@ -8076,7 +8076,7 @@
         <v>90.7</v>
       </c>
       <c r="D124" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.59999999999999432</v>
       </c>
       <c r="E124" s="3">
@@ -8089,7 +8089,7 @@
         <v>31.3</v>
       </c>
       <c r="H124" s="3">
-        <f>G124-F124</f>
+        <f t="shared" si="7"/>
         <v>0.40000000000000213</v>
       </c>
       <c r="I124" s="3">
@@ -8099,7 +8099,7 @@
         <v>28.6</v>
       </c>
       <c r="K124" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.6000000000000014</v>
       </c>
       <c r="L124" s="3">
@@ -8138,7 +8138,7 @@
         <v>109.4</v>
       </c>
       <c r="D125" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="E125" s="3">
@@ -8151,7 +8151,7 @@
         <v>32.700000000000003</v>
       </c>
       <c r="H125" s="3">
-        <f>G125-F125</f>
+        <f t="shared" si="7"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="I125" s="3">
@@ -8161,7 +8161,7 @@
         <v>29.1</v>
       </c>
       <c r="K125" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-2.5999999999999979</v>
       </c>
       <c r="L125" s="3">
@@ -8200,7 +8200,7 @@
         <v>106.5</v>
       </c>
       <c r="D126" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E126" s="3">
@@ -8213,7 +8213,7 @@
         <v>31.5</v>
       </c>
       <c r="H126" s="3">
-        <f>G126-F126</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I126" s="3">
@@ -8223,7 +8223,7 @@
         <v>30.7</v>
       </c>
       <c r="K126" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-4.0000000000000036</v>
       </c>
       <c r="L126" s="3">
@@ -8262,7 +8262,7 @@
         <v>103.9</v>
       </c>
       <c r="D127" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.70000000000000284</v>
       </c>
       <c r="E127" s="3">
@@ -8275,7 +8275,7 @@
         <v>31.4</v>
       </c>
       <c r="H127" s="3">
-        <f>G127-F127</f>
+        <f t="shared" si="7"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I127" s="3">
@@ -8285,7 +8285,7 @@
         <v>29.6</v>
       </c>
       <c r="K127" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.80000000000000071</v>
       </c>
       <c r="L127" s="3">
@@ -8324,7 +8324,7 @@
         <v>96.7</v>
       </c>
       <c r="D128" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.60000000000000853</v>
       </c>
       <c r="E128" s="3">
@@ -8337,7 +8337,7 @@
         <v>33.1</v>
       </c>
       <c r="H128" s="3">
-        <f>G128-F128</f>
+        <f t="shared" si="7"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="I128" s="3">
@@ -8347,7 +8347,7 @@
         <v>29.2</v>
       </c>
       <c r="K128" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-0.30000000000000071</v>
       </c>
       <c r="L128" s="3">
@@ -8386,7 +8386,7 @@
         <v>94</v>
       </c>
       <c r="D129" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="E129" s="3">
@@ -8399,7 +8399,7 @@
         <v>32.1</v>
       </c>
       <c r="H129" s="3">
-        <f>G129-F129</f>
+        <f t="shared" si="7"/>
         <v>0.60000000000000142</v>
       </c>
       <c r="I129" s="3">
@@ -8409,7 +8409,7 @@
         <v>30.7</v>
       </c>
       <c r="K129" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-1.3000000000000007</v>
       </c>
       <c r="L129" s="3">
@@ -8448,7 +8448,7 @@
         <v>91.1</v>
       </c>
       <c r="D130" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.1999999999999886</v>
       </c>
       <c r="E130" s="3">
@@ -8461,7 +8461,7 @@
         <v>28.8</v>
       </c>
       <c r="H130" s="3">
-        <f>G130-F130</f>
+        <f t="shared" ref="H130:H161" si="8">G130-F130</f>
         <v>0.40000000000000213</v>
       </c>
       <c r="I130" s="3">
@@ -8471,7 +8471,7 @@
         <v>28.3</v>
       </c>
       <c r="K130" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="L130" s="3">
@@ -8510,7 +8510,7 @@
         <v>102.9</v>
       </c>
       <c r="D131" s="3">
-        <f t="shared" ref="D131:D137" si="4">C131-B131</f>
+        <f t="shared" ref="D131:D137" si="9">C131-B131</f>
         <v>-1.2999999999999972</v>
       </c>
       <c r="E131" s="3">
@@ -8523,7 +8523,7 @@
         <v>27</v>
       </c>
       <c r="H131" s="3">
-        <f>G131-F131</f>
+        <f t="shared" si="8"/>
         <v>0.19999999999999929</v>
       </c>
       <c r="I131" s="3">
@@ -8533,7 +8533,7 @@
         <v>20.3</v>
       </c>
       <c r="K131" s="3">
-        <f t="shared" ref="K131:K137" si="5">J131-I131</f>
+        <f t="shared" ref="K131:K137" si="10">J131-I131</f>
         <v>-3.3000000000000007</v>
       </c>
       <c r="L131" s="3">
@@ -8572,7 +8572,7 @@
         <v>92.7</v>
       </c>
       <c r="D132" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-0.20000000000000284</v>
       </c>
       <c r="E132" s="3">
@@ -8585,7 +8585,7 @@
         <v>29.3</v>
       </c>
       <c r="H132" s="3">
-        <f>G132-F132</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I132" s="3">
@@ -8595,7 +8595,7 @@
         <v>25.1</v>
       </c>
       <c r="K132" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="L132" s="3">
@@ -8634,7 +8634,7 @@
         <v>90.3</v>
       </c>
       <c r="D133" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-0.79999999999999716</v>
       </c>
       <c r="E133" s="3">
@@ -8647,7 +8647,7 @@
         <v>26.7</v>
       </c>
       <c r="H133" s="3">
-        <f>G133-F133</f>
+        <f t="shared" si="8"/>
         <v>-0.19999999999999929</v>
       </c>
       <c r="I133" s="3">
@@ -8657,7 +8657,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="K133" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-2.5</v>
       </c>
       <c r="L133" s="3">
@@ -8696,7 +8696,7 @@
         <v>108</v>
       </c>
       <c r="D134" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-9.9999999999994316E-2</v>
       </c>
       <c r="E134" s="3">
@@ -8709,7 +8709,7 @@
         <v>34.1</v>
       </c>
       <c r="H134" s="3">
-        <f>G134-F134</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I134" s="3">
@@ -8719,7 +8719,7 @@
         <v>34.6</v>
       </c>
       <c r="K134" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-2.1000000000000014</v>
       </c>
       <c r="L134" s="3">
@@ -8758,7 +8758,7 @@
         <v>101.4</v>
       </c>
       <c r="D135" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>1.6000000000000085</v>
       </c>
       <c r="E135" s="3">
@@ -8771,7 +8771,7 @@
         <v>34.299999999999997</v>
       </c>
       <c r="H135" s="3">
-        <f>G135-F135</f>
+        <f t="shared" si="8"/>
         <v>0.59999999999999432</v>
       </c>
       <c r="I135" s="3">
@@ -8781,7 +8781,7 @@
         <v>36.700000000000003</v>
       </c>
       <c r="K135" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-0.79999999999999716</v>
       </c>
       <c r="L135" s="3">
@@ -8820,7 +8820,7 @@
         <v>93.9</v>
       </c>
       <c r="D136" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-2.1999999999999886</v>
       </c>
       <c r="E136" s="3">
@@ -8833,7 +8833,7 @@
         <v>32.9</v>
       </c>
       <c r="H136" s="3">
-        <f>G136-F136</f>
+        <f t="shared" si="8"/>
         <v>-0.70000000000000284</v>
       </c>
       <c r="I136" s="3">
@@ -8843,7 +8843,7 @@
         <v>27.4</v>
       </c>
       <c r="K136" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>-1.4000000000000021</v>
       </c>
       <c r="L136" s="3">
@@ -8882,7 +8882,7 @@
         <v>70.7</v>
       </c>
       <c r="D137" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-1.2000000000000028</v>
       </c>
       <c r="E137" s="3">
@@ -8895,7 +8895,7 @@
         <v>25</v>
       </c>
       <c r="H137" s="3">
-        <f>G137-F137</f>
+        <f t="shared" si="8"/>
         <v>-0.5</v>
       </c>
       <c r="I137" s="3">
@@ -8905,7 +8905,7 @@
         <v>26.4</v>
       </c>
       <c r="K137" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
       <c r="L137" s="3">

</xml_diff>